<commit_message>
Update ReadExcel File Code
</commit_message>
<xml_diff>
--- a/Files/ExcelWriteRead.xlsx
+++ b/Files/ExcelWriteRead.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,39 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
-    <t>This is Row No 0 and col no 0</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 1</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 2</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 3</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 4</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 5</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 6</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 7</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 8</t>
-  </si>
-  <si>
-    <t>This is Row No 0 and col no 9</t>
-  </si>
-  <si>
-    <t>This is Row No 1 and col no 0</t>
-  </si>
-  <si>
     <t>This is Row No 1 and col no 1</t>
   </si>
   <si>
@@ -81,7 +48,7 @@
     <t>This is Row No 1 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 2 and col no 0</t>
+    <t>This is Row No 1 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 2 and col no 1</t>
@@ -111,7 +78,7 @@
     <t>This is Row No 2 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 3 and col no 0</t>
+    <t>This is Row No 2 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 3 and col no 1</t>
@@ -141,7 +108,7 @@
     <t>This is Row No 3 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 4 and col no 0</t>
+    <t>This is Row No 3 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 4 and col no 1</t>
@@ -171,7 +138,7 @@
     <t>This is Row No 4 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 5 and col no 0</t>
+    <t>This is Row No 4 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 5 and col no 1</t>
@@ -201,7 +168,7 @@
     <t>This is Row No 5 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 6 and col no 0</t>
+    <t>This is Row No 5 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 6 and col no 1</t>
@@ -231,7 +198,7 @@
     <t>This is Row No 6 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 7 and col no 0</t>
+    <t>This is Row No 6 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 7 and col no 1</t>
@@ -261,7 +228,7 @@
     <t>This is Row No 7 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 8 and col no 0</t>
+    <t>This is Row No 7 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 8 and col no 1</t>
@@ -291,7 +258,7 @@
     <t>This is Row No 8 and col no 9</t>
   </si>
   <si>
-    <t>This is Row No 9 and col no 0</t>
+    <t>This is Row No 8 and col no 10</t>
   </si>
   <si>
     <t>This is Row No 9 and col no 1</t>
@@ -319,12 +286,46 @@
   </si>
   <si>
     <t>This is Row No 9 and col no 9</t>
+  </si>
+  <si>
+    <t>This is Row No 9 and col no 10</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 1</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 2</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 3</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 4</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 5</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 6</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 7</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 8</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 9</t>
+  </si>
+  <si>
+    <t>This is Row No 10 and col no 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,12 +640,12 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -708,7 +709,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -740,7 +741,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -772,7 +773,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -804,7 +805,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -836,7 +837,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -868,7 +869,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -900,7 +901,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -932,7 +933,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>90</v>
       </c>

</xml_diff>